<commit_message>
✨ [feat] se insertaron cambios
</commit_message>
<xml_diff>
--- a/formatos/Jornada Laboral.xlsx
+++ b/formatos/Jornada Laboral.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eperez\Desktop\Sistema Amaxonia\Info Sist RH\2025-03-21\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eperez\Desktop\Sistema Amaxonia\Info Sist RH\2025-06-09\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{26587D65-8B71-44C9-BFFE-6CE5AFE604D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF5EC0F4-24FD-402E-B8AE-9C5EFB0D42D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{62C3D3AB-C08B-4424-B134-BCCB9599987F}"/>
+    <workbookView xWindow="-24120" yWindow="2610" windowWidth="24240" windowHeight="13020" xr2:uid="{19FD0B20-1F65-4250-8E69-274540BAF54D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -258,8 +258,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -287,8 +295,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -622,93 +631,93 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B1D1A28-A063-41D9-8CDB-7CA0D6489AFD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4490DF98-F402-48C3-AE3C-6E755BB20E5D}">
   <dimension ref="A1:AA45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>